<commit_message>
Updated the power and energy density values for the army goal in the excel workbook with the data. -Tom 03/22/2023
</commit_message>
<xml_diff>
--- a/include/Li_ion_battery_figure.xlsx
+++ b/include/Li_ion_battery_figure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasdonahue/Desktop/Classes/Research/Li-Ion-Visualizer/include/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D30A912-D232-B345-AD41-4207EDD1CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC072B7C-BDA6-AE48-AA65-B4BF6ACB72CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="1580" windowWidth="23200" windowHeight="13780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2144,10 +2144,10 @@
         <v>2025</v>
       </c>
       <c r="B68" s="2">
-        <v>227.27</v>
+        <v>326</v>
       </c>
       <c r="C68" s="2">
-        <v>2272.7199999999998</v>
+        <v>2333.3330000000001</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>71</v>

</xml_diff>